<commit_message>
corrected few mistakes with taxonomy mixing between primers
</commit_message>
<xml_diff>
--- a/data/raw-data/2024.11.10_16Smam_eDNA_abundance_samplecorrected.xlsx
+++ b/data/raw-data/2024.11.10_16Smam_eDNA_abundance_samplecorrected.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aloïsito\Documents\Nextcloud\MyDrive\2024 11 04 _teletravailling avant pyrennes\00_Papier_substrats\raw_data (pour diffusion)\data_used_for_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berardal\Documents\Aloïs\BePrep\00_Papier_substrats\raw_data (pour diffusion)\data_used_for_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D41D7DC-27D2-4918-9730-D4A66302E903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Merge_taxa (2)" sheetId="7" r:id="rId1"/>
@@ -2135,7 +2134,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0E+00"/>
   </numFmts>
@@ -3028,14 +3027,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:NW51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="18" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="S1" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD13"/>
+      <selection pane="bottomRight" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -36883,7 +36882,7 @@
         <v>698</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>603</v>
+        <v>698</v>
       </c>
       <c r="J30" s="6"/>
       <c r="K30" t="s">

</xml_diff>